<commit_message>
fixing the problem with exporting the excel file
</commit_message>
<xml_diff>
--- a/uploads/invoice-template.xlsx
+++ b/uploads/invoice-template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\inha-accounting.local\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OSPanel\domains\inha-accounting.local\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7170"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7170"/>
   </bookViews>
   <sheets>
     <sheet name="821" sheetId="1" r:id="rId1"/>
@@ -1222,32 +1222,20 @@
   <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
@@ -1256,65 +1244,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1327,201 +1261,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="4" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="4" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="4" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1543,20 +1309,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="justify"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1566,9 +1323,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1576,27 +1330,12 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1605,107 +1344,14 @@
     <xf numFmtId="2" fontId="1" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="59" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="60" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="61" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="62" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="63" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="64" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="65" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="66" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="67" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="68" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="69" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="66" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="67" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1713,10 +1359,364 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="59" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="60" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="61" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="68" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="62" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="63" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="64" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="69" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="66" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="67" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="65" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="66" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="67" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="4" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="4" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="4" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1798,9 +1798,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1838,7 +1838,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1910,7 +1910,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2067,679 +2067,679 @@
   <dimension ref="B1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="0.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="25" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13" style="6" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="4.85546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="21.85546875" style="6" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="0.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="25" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3">
+      <c r="D1" s="174"/>
+      <c r="E1" s="2">
         <f>'[1]Reg.List'!I6</f>
         <v>2685</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="175">
         <f>'[1]Reg.List'!J6</f>
         <v>43251</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="H1" s="175"/>
+      <c r="I1" s="175"/>
+      <c r="J1" s="175"/>
+      <c r="K1" s="175"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="2:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9" t="str">
+      <c r="D3" s="61"/>
+      <c r="E3" s="6" t="str">
         <f>'[1]Reg.List'!E6</f>
         <v>SOCIE 2017/096</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="175">
         <f>'[1]Reg.List'!G6</f>
         <v>42963</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="175"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:12" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="B4" s="176"/>
+      <c r="C4" s="176"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="176"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="176"/>
+      <c r="H4" s="176"/>
+      <c r="I4" s="176"/>
+      <c r="J4" s="176"/>
+      <c r="K4" s="176"/>
+      <c r="L4" s="176"/>
     </row>
     <row r="5" spans="2:12" ht="5.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="14"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="177" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="15" t="s">
+      <c r="D6" s="177"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="19"/>
+      <c r="G6" s="178"/>
+      <c r="H6" s="178"/>
+      <c r="I6" s="178"/>
+      <c r="J6" s="178"/>
+      <c r="K6" s="178"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="172" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="15" t="s">
+      <c r="D7" s="172"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="19"/>
+      <c r="G7" s="161"/>
+      <c r="H7" s="161"/>
+      <c r="I7" s="161"/>
+      <c r="J7" s="161"/>
+      <c r="K7" s="161"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="172" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="15" t="s">
+      <c r="D8" s="172"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="19"/>
+      <c r="G8" s="161"/>
+      <c r="H8" s="161"/>
+      <c r="I8" s="161"/>
+      <c r="J8" s="161"/>
+      <c r="K8" s="161"/>
+      <c r="L8" s="13"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="160" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="15" t="s">
+      <c r="D9" s="160"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="19"/>
+      <c r="G9" s="161"/>
+      <c r="H9" s="161"/>
+      <c r="I9" s="161"/>
+      <c r="J9" s="161"/>
+      <c r="K9" s="161"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="172" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="15" t="s">
+      <c r="D10" s="172"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="19"/>
+      <c r="G10" s="161"/>
+      <c r="H10" s="161"/>
+      <c r="I10" s="161"/>
+      <c r="J10" s="161"/>
+      <c r="K10" s="161"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="160" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="15" t="s">
+      <c r="D11" s="160"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="19"/>
+      <c r="G11" s="161"/>
+      <c r="H11" s="161"/>
+      <c r="I11" s="161"/>
+      <c r="J11" s="161"/>
+      <c r="K11" s="161"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="15" t="s">
+      <c r="D12" s="173"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="19"/>
+      <c r="G12" s="161"/>
+      <c r="H12" s="161"/>
+      <c r="I12" s="161"/>
+      <c r="J12" s="161"/>
+      <c r="K12" s="161"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="15" t="s">
+      <c r="D13" s="160"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="19"/>
+      <c r="G13" s="161"/>
+      <c r="H13" s="161"/>
+      <c r="I13" s="161"/>
+      <c r="J13" s="161"/>
+      <c r="K13" s="161"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="2:12" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="26"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="16"/>
     </row>
     <row r="15" spans="2:12" ht="6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:12" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="162" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29" t="s">
+      <c r="C16" s="163"/>
+      <c r="D16" s="129" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="166" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="162" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="168" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="H16" s="170" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33" t="s">
+      <c r="I16" s="171"/>
+      <c r="J16" s="171" t="s">
         <v>26</v>
       </c>
-      <c r="K16" s="28"/>
-      <c r="L16" s="29" t="s">
+      <c r="K16" s="163"/>
+      <c r="L16" s="129" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="39" t="s">
+      <c r="B17" s="164"/>
+      <c r="C17" s="165"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="167"/>
+      <c r="F17" s="164"/>
+      <c r="G17" s="169"/>
+      <c r="H17" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="40" t="s">
+      <c r="I17" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="41" t="s">
+      <c r="J17" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="42" t="s">
+      <c r="K17" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="L17" s="36"/>
+      <c r="L17" s="130"/>
     </row>
     <row r="18" spans="2:14" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="43">
+      <c r="B18" s="131">
         <v>1</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45">
+      <c r="C18" s="132"/>
+      <c r="D18" s="21">
         <v>2</v>
       </c>
-      <c r="E18" s="46">
+      <c r="E18" s="22">
         <v>3</v>
       </c>
-      <c r="F18" s="47">
+      <c r="F18" s="23">
         <v>4</v>
       </c>
-      <c r="G18" s="48">
+      <c r="G18" s="24">
         <v>5</v>
       </c>
-      <c r="H18" s="49">
+      <c r="H18" s="25">
         <v>6</v>
       </c>
-      <c r="I18" s="50">
+      <c r="I18" s="26">
         <v>7</v>
       </c>
-      <c r="J18" s="50">
+      <c r="J18" s="26">
         <v>8</v>
       </c>
-      <c r="K18" s="51">
+      <c r="K18" s="27">
         <v>9</v>
       </c>
-      <c r="L18" s="45">
+      <c r="L18" s="21">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="133" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54" t="s">
+      <c r="C19" s="134"/>
+      <c r="D19" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="55"/>
-      <c r="F19" s="56">
+      <c r="E19" s="138"/>
+      <c r="F19" s="141">
         <f>'[1]Reg.List'!K6</f>
         <v>10525875</v>
       </c>
-      <c r="G19" s="57">
+      <c r="G19" s="144">
         <f>F19</f>
         <v>10525875</v>
       </c>
-      <c r="H19" s="58" t="s">
+      <c r="H19" s="147" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="59"/>
-      <c r="J19" s="60" t="s">
+      <c r="I19" s="148"/>
+      <c r="J19" s="153" t="s">
         <v>33</v>
       </c>
-      <c r="K19" s="61"/>
-      <c r="L19" s="62" t="s">
+      <c r="K19" s="154"/>
+      <c r="L19" s="159" t="s">
         <v>34</v>
       </c>
-      <c r="N19" s="63"/>
+      <c r="N19" s="28"/>
     </row>
     <row r="20" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="64" t="str">
+      <c r="B20" s="106" t="str">
         <f>'[1]Reg.List'!B6</f>
         <v>SHOKHUJAEV IBROKHIMKHUJA</v>
       </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="70"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="74"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="136"/>
+      <c r="E20" s="139"/>
+      <c r="F20" s="142"/>
+      <c r="G20" s="145"/>
+      <c r="H20" s="149"/>
+      <c r="I20" s="150"/>
+      <c r="J20" s="155"/>
+      <c r="K20" s="156"/>
+      <c r="L20" s="108"/>
     </row>
     <row r="21" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="76" t="str">
+      <c r="C21" s="30" t="str">
         <f>'[1]Reg.List'!C6</f>
         <v>SOCIE</v>
       </c>
-      <c r="D21" s="66"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="73"/>
-      <c r="L21" s="74" t="s">
+      <c r="D21" s="136"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="142"/>
+      <c r="G21" s="145"/>
+      <c r="H21" s="149"/>
+      <c r="I21" s="150"/>
+      <c r="J21" s="155"/>
+      <c r="K21" s="156"/>
+      <c r="L21" s="108" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="77" t="str">
+      <c r="B22" s="110" t="str">
         <f>'[1]Reg.List'!D5</f>
         <v xml:space="preserve"> за II-семестр 2017 / 2018 учеб. год</v>
       </c>
-      <c r="C22" s="78"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="82"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="85"/>
-      <c r="K22" s="86"/>
-      <c r="L22" s="87"/>
+      <c r="C22" s="111"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="140"/>
+      <c r="F22" s="143"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="151"/>
+      <c r="I22" s="152"/>
+      <c r="J22" s="157"/>
+      <c r="K22" s="158"/>
+      <c r="L22" s="109"/>
     </row>
     <row r="23" spans="2:14" ht="9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="88"/>
-      <c r="C23" s="89"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="89"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="89"/>
-      <c r="I23" s="89"/>
-      <c r="J23" s="89"/>
-      <c r="K23" s="89"/>
-      <c r="L23" s="90"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="113"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="113"/>
+      <c r="K23" s="113"/>
+      <c r="L23" s="114"/>
     </row>
     <row r="24" spans="2:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="91" t="s">
+      <c r="B24" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="92"/>
-      <c r="D24" s="93" t="s">
+      <c r="C24" s="98"/>
+      <c r="D24" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="94"/>
-      <c r="F24" s="95">
+      <c r="E24" s="119"/>
+      <c r="F24" s="121">
         <f>F19</f>
         <v>10525875</v>
       </c>
-      <c r="G24" s="96">
+      <c r="G24" s="123">
         <f>G19</f>
         <v>10525875</v>
       </c>
-      <c r="H24" s="97" t="s">
+      <c r="H24" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="I24" s="98"/>
-      <c r="J24" s="99" t="s">
+      <c r="I24" s="126"/>
+      <c r="J24" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="92"/>
-      <c r="L24" s="100" t="s">
+      <c r="K24" s="98"/>
+      <c r="L24" s="31" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="101"/>
-      <c r="C25" s="102"/>
-      <c r="D25" s="103"/>
-      <c r="E25" s="104"/>
-      <c r="F25" s="105"/>
-      <c r="G25" s="106"/>
-      <c r="H25" s="107"/>
-      <c r="I25" s="108"/>
-      <c r="J25" s="109"/>
-      <c r="K25" s="102"/>
-      <c r="L25" s="110" t="s">
+      <c r="B25" s="116"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="120"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="124"/>
+      <c r="H25" s="127"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="99"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:14" ht="7.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="111"/>
-      <c r="C26" s="112"/>
-      <c r="D26" s="113"/>
-      <c r="E26" s="113"/>
-      <c r="F26" s="113"/>
-      <c r="G26" s="113"/>
-      <c r="H26" s="113"/>
-      <c r="I26" s="113"/>
-      <c r="J26" s="113"/>
-      <c r="K26" s="113"/>
-      <c r="L26" s="114"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="36"/>
     </row>
     <row r="27" spans="2:14" ht="4.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="115"/>
-      <c r="C27" s="115"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="116"/>
-      <c r="F27" s="116"/>
-      <c r="G27" s="116"/>
-      <c r="H27" s="116"/>
-      <c r="I27" s="116"/>
-      <c r="J27" s="116"/>
-      <c r="K27" s="116"/>
-      <c r="L27" s="116"/>
+      <c r="B27" s="101"/>
+      <c r="C27" s="101"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
     </row>
     <row r="28" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="116"/>
-      <c r="C28" s="116"/>
-      <c r="D28" s="116"/>
-      <c r="E28" s="116"/>
-      <c r="F28" s="116"/>
-      <c r="G28" s="117"/>
-      <c r="H28" s="118"/>
-      <c r="I28" s="118"/>
-      <c r="J28" s="118"/>
-      <c r="K28" s="116"/>
-      <c r="L28" s="116"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="102"/>
+      <c r="I28" s="102"/>
+      <c r="J28" s="102"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="119" t="s">
+      <c r="B29" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="120" t="e">
+      <c r="C29" s="103" t="e">
         <f ca="1">[2]!prop(F24)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D29" s="120"/>
-      <c r="E29" s="120"/>
-      <c r="F29" s="120"/>
-      <c r="G29" s="120"/>
-      <c r="H29" s="120"/>
-      <c r="I29" s="120"/>
-      <c r="J29" s="120"/>
-      <c r="K29" s="120"/>
-      <c r="L29" s="120"/>
+      <c r="D29" s="103"/>
+      <c r="E29" s="103"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="103"/>
+      <c r="J29" s="103"/>
+      <c r="K29" s="103"/>
+      <c r="L29" s="103"/>
     </row>
     <row r="30" spans="2:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="116"/>
-      <c r="C30" s="116"/>
-      <c r="D30" s="116"/>
-      <c r="E30" s="116"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
-      <c r="H30" s="116"/>
-      <c r="I30" s="116"/>
-      <c r="J30" s="116"/>
-      <c r="K30" s="116"/>
-      <c r="L30" s="116"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B31" s="116"/>
-      <c r="C31" s="116"/>
-      <c r="D31" s="116"/>
-      <c r="E31" s="116"/>
-      <c r="F31" s="116"/>
-      <c r="G31" s="121" t="s">
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="122"/>
-      <c r="I31" s="122"/>
-      <c r="J31" s="122"/>
-      <c r="K31" s="122"/>
-      <c r="L31" s="122"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="41"/>
     </row>
     <row r="32" spans="2:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="B32" s="123" t="s">
+      <c r="B32" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="116"/>
-      <c r="D32" s="124" t="s">
+      <c r="C32" s="37"/>
+      <c r="D32" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="115"/>
-      <c r="F32" s="116"/>
-      <c r="G32" s="125" t="s">
+      <c r="E32" s="101"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="H32" s="126"/>
-      <c r="I32" s="126"/>
-      <c r="J32" s="126"/>
-      <c r="K32" s="126"/>
-      <c r="L32" s="126"/>
-      <c r="N32" s="127"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="44"/>
+      <c r="N32" s="45"/>
     </row>
     <row r="33" spans="2:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="116"/>
-      <c r="C33" s="116"/>
-      <c r="D33" s="116"/>
-      <c r="E33" s="116"/>
-      <c r="F33" s="116"/>
-      <c r="G33" s="123" t="s">
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="H33" s="116"/>
-      <c r="I33" s="116"/>
-      <c r="J33" s="116"/>
-      <c r="K33" s="116"/>
-      <c r="L33" s="116"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
     </row>
     <row r="34" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="123" t="s">
+      <c r="B34" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="116"/>
-      <c r="D34" s="115" t="s">
+      <c r="C34" s="37"/>
+      <c r="D34" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="115"/>
-      <c r="F34" s="116"/>
-      <c r="G34" s="128" t="s">
+      <c r="E34" s="101"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="H34" s="128"/>
-      <c r="I34" s="128"/>
-      <c r="J34" s="128"/>
-      <c r="K34" s="128"/>
-      <c r="L34" s="128"/>
+      <c r="H34" s="105"/>
+      <c r="I34" s="105"/>
+      <c r="J34" s="105"/>
+      <c r="K34" s="105"/>
+      <c r="L34" s="105"/>
     </row>
     <row r="35" spans="2:12" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="116" t="s">
+      <c r="B35" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="116"/>
-      <c r="D35" s="116"/>
-      <c r="E35" s="116"/>
-      <c r="F35" s="116"/>
-      <c r="H35" s="129"/>
-      <c r="I35" s="129"/>
-      <c r="J35" s="129"/>
-      <c r="K35" s="129"/>
-      <c r="L35" s="129"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B36" s="123"/>
-      <c r="H36" s="130" t="s">
+      <c r="B36" s="42"/>
+      <c r="H36" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="I36" s="130"/>
-      <c r="J36" s="130"/>
-      <c r="K36" s="130"/>
-      <c r="L36" s="130"/>
+      <c r="I36" s="92"/>
+      <c r="J36" s="92"/>
+      <c r="K36" s="92"/>
+      <c r="L36" s="92"/>
     </row>
     <row r="37" spans="2:12" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="131"/>
-      <c r="C37" s="131"/>
-      <c r="H37" s="132"/>
-      <c r="I37" s="132"/>
-      <c r="J37" s="132"/>
-      <c r="K37" s="132"/>
-      <c r="L37" s="132"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="93"/>
+      <c r="H37" s="94"/>
+      <c r="I37" s="94"/>
+      <c r="J37" s="94"/>
+      <c r="K37" s="94"/>
+      <c r="L37" s="94"/>
     </row>
     <row r="38" spans="2:12" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="133"/>
-      <c r="C38" s="133"/>
-      <c r="H38" s="134"/>
-      <c r="I38" s="134"/>
-      <c r="J38" s="134"/>
-      <c r="K38" s="134"/>
-      <c r="L38" s="134"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="48"/>
+      <c r="L38" s="48"/>
     </row>
     <row r="39" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="135" t="s">
+      <c r="B40" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="135"/>
-      <c r="D40" s="135"/>
-      <c r="E40" s="135"/>
-      <c r="F40" s="135"/>
-      <c r="G40" s="136">
+      <c r="C40" s="95"/>
+      <c r="D40" s="95"/>
+      <c r="E40" s="95"/>
+      <c r="F40" s="95"/>
+      <c r="G40" s="49">
         <f>E1</f>
         <v>2685</v>
       </c>
@@ -2750,246 +2750,257 @@
       <c r="L40" s="1"/>
     </row>
     <row r="41" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="137"/>
-      <c r="C41" s="8" t="s">
+      <c r="B41" s="50"/>
+      <c r="C41" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="138" t="str">
+      <c r="D41" s="61"/>
+      <c r="E41" s="51" t="str">
         <f>E3</f>
         <v>SOCIE 2017/096</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G41" s="139">
+      <c r="G41" s="96">
         <f>G3</f>
         <v>42963</v>
       </c>
-      <c r="H41" s="139"/>
+      <c r="H41" s="96"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="137"/>
-      <c r="L41" s="137"/>
+      <c r="K41" s="50"/>
+      <c r="L41" s="50"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B43" s="140" t="s">
+      <c r="B43" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="140"/>
-      <c r="D43" s="140"/>
-      <c r="E43" s="140"/>
-      <c r="F43" s="140"/>
-      <c r="G43" s="140"/>
-      <c r="H43" s="140"/>
-      <c r="I43" s="140"/>
-      <c r="J43" s="141">
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="83">
         <f>G1</f>
         <v>43251</v>
       </c>
-      <c r="K43" s="142"/>
-      <c r="L43" s="142"/>
+      <c r="K43" s="84"/>
+      <c r="L43" s="84"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B45" s="143" t="s">
+      <c r="B45" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="143"/>
-      <c r="D45" s="143"/>
-      <c r="E45" s="143"/>
-      <c r="F45" s="143"/>
-      <c r="G45" s="143"/>
-      <c r="H45" s="143"/>
-      <c r="I45" s="143"/>
-      <c r="J45" s="143"/>
-      <c r="K45" s="143"/>
-      <c r="L45" s="143"/>
+      <c r="C45" s="85"/>
+      <c r="D45" s="85"/>
+      <c r="E45" s="85"/>
+      <c r="F45" s="85"/>
+      <c r="G45" s="85"/>
+      <c r="H45" s="85"/>
+      <c r="I45" s="85"/>
+      <c r="J45" s="85"/>
+      <c r="K45" s="85"/>
+      <c r="L45" s="85"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B46" s="144" t="s">
+      <c r="B46" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="144"/>
-      <c r="D46" s="145"/>
-      <c r="E46" s="145"/>
-      <c r="F46" s="145"/>
-      <c r="G46" s="145"/>
-      <c r="H46" s="145"/>
-      <c r="I46" s="145"/>
-      <c r="J46" s="145"/>
-      <c r="K46" s="145"/>
-      <c r="L46" s="145"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="86"/>
+      <c r="G46" s="86"/>
+      <c r="H46" s="86"/>
+      <c r="I46" s="86"/>
+      <c r="J46" s="86"/>
+      <c r="K46" s="86"/>
+      <c r="L46" s="86"/>
     </row>
     <row r="47" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="146" t="s">
+      <c r="B47" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="146"/>
-      <c r="D47" s="146"/>
-      <c r="E47" s="146"/>
-      <c r="F47" s="146"/>
-      <c r="G47" s="146"/>
-      <c r="H47" s="146"/>
-      <c r="I47" s="146"/>
-      <c r="J47" s="146"/>
-      <c r="K47" s="146"/>
-      <c r="L47" s="146"/>
+      <c r="C47" s="87"/>
+      <c r="D47" s="87"/>
+      <c r="E47" s="87"/>
+      <c r="F47" s="87"/>
+      <c r="G47" s="87"/>
+      <c r="H47" s="87"/>
+      <c r="I47" s="87"/>
+      <c r="J47" s="87"/>
+      <c r="K47" s="87"/>
+      <c r="L47" s="87"/>
     </row>
     <row r="48" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="147" t="s">
+      <c r="B49" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="C49" s="148"/>
-      <c r="D49" s="148"/>
-      <c r="E49" s="148"/>
-      <c r="F49" s="149"/>
-      <c r="G49" s="147" t="s">
+      <c r="C49" s="89"/>
+      <c r="D49" s="89"/>
+      <c r="E49" s="89"/>
+      <c r="F49" s="90"/>
+      <c r="G49" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="H49" s="148"/>
-      <c r="I49" s="148" t="s">
+      <c r="H49" s="89"/>
+      <c r="I49" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="J49" s="148"/>
-      <c r="K49" s="150"/>
-      <c r="L49" s="151"/>
+      <c r="J49" s="89"/>
+      <c r="K49" s="91"/>
+      <c r="L49" s="54"/>
     </row>
     <row r="50" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="152" t="s">
+      <c r="B50" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="153" t="str">
+      <c r="C50" s="64" t="str">
         <f>B20</f>
         <v>SHOKHUJAEV IBROKHIMKHUJA</v>
       </c>
-      <c r="D50" s="153"/>
-      <c r="E50" s="153"/>
-      <c r="F50" s="154"/>
-      <c r="G50" s="155" t="s">
+      <c r="D50" s="64"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="65"/>
+      <c r="G50" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="H50" s="156"/>
-      <c r="I50" s="157">
+      <c r="H50" s="67"/>
+      <c r="I50" s="70">
         <f>F19</f>
         <v>10525875</v>
       </c>
-      <c r="J50" s="158"/>
-      <c r="K50" s="159"/>
-      <c r="L50" s="160"/>
+      <c r="J50" s="71"/>
+      <c r="K50" s="72"/>
+      <c r="L50" s="56"/>
     </row>
     <row r="51" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="161" t="s">
+      <c r="B51" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="C51" s="162"/>
-      <c r="D51" s="162"/>
-      <c r="E51" s="162"/>
-      <c r="F51" s="163"/>
-      <c r="G51" s="164"/>
-      <c r="H51" s="165"/>
-      <c r="I51" s="166"/>
-      <c r="J51" s="167"/>
-      <c r="K51" s="168"/>
+      <c r="C51" s="77"/>
+      <c r="D51" s="77"/>
+      <c r="E51" s="77"/>
+      <c r="F51" s="78"/>
+      <c r="G51" s="68"/>
+      <c r="H51" s="69"/>
+      <c r="I51" s="73"/>
+      <c r="J51" s="74"/>
+      <c r="K51" s="75"/>
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="169"/>
-      <c r="C52" s="170"/>
-      <c r="D52" s="170"/>
-      <c r="E52" s="170"/>
-      <c r="F52" s="171"/>
-      <c r="G52" s="169"/>
-      <c r="H52" s="170"/>
-      <c r="I52" s="170"/>
-      <c r="J52" s="170"/>
-      <c r="K52" s="172"/>
-      <c r="L52" s="173"/>
+      <c r="B52" s="79"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="80"/>
+      <c r="E52" s="80"/>
+      <c r="F52" s="81"/>
+      <c r="G52" s="79"/>
+      <c r="H52" s="80"/>
+      <c r="I52" s="80"/>
+      <c r="J52" s="80"/>
+      <c r="K52" s="82"/>
+      <c r="L52" s="57"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="174" t="e">
+      <c r="C54" s="61"/>
+      <c r="D54" s="62" t="e">
         <f ca="1">C29</f>
         <v>#NAME?</v>
       </c>
-      <c r="E54" s="174"/>
-      <c r="F54" s="174"/>
-      <c r="G54" s="174"/>
-      <c r="H54" s="174"/>
-      <c r="I54" s="174"/>
-      <c r="J54" s="174"/>
-      <c r="K54" s="174"/>
-      <c r="L54" s="174"/>
+      <c r="E54" s="62"/>
+      <c r="F54" s="62"/>
+      <c r="G54" s="62"/>
+      <c r="H54" s="62"/>
+      <c r="I54" s="62"/>
+      <c r="J54" s="62"/>
+      <c r="K54" s="62"/>
+      <c r="L54" s="62"/>
     </row>
     <row r="55" spans="2:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="175" t="s">
+      <c r="B55" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="175"/>
-      <c r="D55" s="175"/>
-      <c r="E55" s="175"/>
-      <c r="F55" s="175"/>
-      <c r="G55" s="175"/>
-      <c r="H55" s="175"/>
-      <c r="I55" s="175"/>
-      <c r="J55" s="175"/>
-      <c r="K55" s="175"/>
-      <c r="L55" s="175"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="63"/>
+      <c r="E55" s="63"/>
+      <c r="F55" s="63"/>
+      <c r="G55" s="63"/>
+      <c r="H55" s="63"/>
+      <c r="I55" s="63"/>
+      <c r="J55" s="63"/>
+      <c r="K55" s="63"/>
+      <c r="L55" s="63"/>
     </row>
     <row r="58" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="C58" s="176" t="s">
+      <c r="C58" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="D58" s="177"/>
-      <c r="E58" s="177"/>
-      <c r="G58" s="178" t="s">
+      <c r="D58" s="59"/>
+      <c r="E58" s="59"/>
+      <c r="G58" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="H58" s="129"/>
-      <c r="I58" s="129"/>
-      <c r="J58" s="129"/>
-      <c r="K58" s="129"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
+      <c r="J58" s="46"/>
+      <c r="K58" s="46"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C59" s="63" t="s">
+      <c r="C59" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="H59" s="6" t="s">
+      <c r="H59" s="4" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:L54"/>
-    <mergeCell ref="B55:L55"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="G50:H51"/>
-    <mergeCell ref="I50:K51"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="G52:K52"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="D46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:K49"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="J24:K25"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="C29:L29"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H19:I22"/>
+    <mergeCell ref="J19:K22"/>
+    <mergeCell ref="L19:L20"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="G34:L34"/>
     <mergeCell ref="B20:C20"/>
@@ -3002,44 +3013,33 @@
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="H24:I25"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="H19:I22"/>
-    <mergeCell ref="J19:K22"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="J24:K25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="C29:L29"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="D46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:L54"/>
+    <mergeCell ref="B55:L55"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="G50:H51"/>
+    <mergeCell ref="I50:K51"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="G52:K52"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="11" scale="53" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Testing upload file and parsing the excel file
</commit_message>
<xml_diff>
--- a/uploads/invoice-template.xlsx
+++ b/uploads/invoice-template.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OSPanel\domains\inha-accounting.local\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\inha-accounting.local\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7170"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7170"/>
   </bookViews>
   <sheets>
     <sheet name="821" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
-    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
@@ -329,37 +328,13 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="70">
     <border>
@@ -1219,21 +1194,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="justify"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1337,13 +1306,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="1" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1359,21 +1322,243 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="59" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="60" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1385,33 +1570,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="68" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="62" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="63" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="64" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="69" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="66" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="67" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="65" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="66" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="67" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1425,298 +1583,107 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="60" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="66" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="67" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="62" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="63" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="64" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="69" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="66" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="67" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="4" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="4" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="4" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1735,72 +1702,26 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Reg.List"/>
-      <sheetName val="821"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="5">
-          <cell r="D5" t="str">
-            <v xml:space="preserve"> за II-семестр 2017 / 2018 учеб. год</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v>SHOKHUJAEV IBROKHIMKHUJA</v>
-          </cell>
-          <cell r="C6" t="str">
-            <v>SOCIE</v>
-          </cell>
-          <cell r="E6" t="str">
-            <v>SOCIE 2017/096</v>
-          </cell>
-          <cell r="G6">
-            <v>42963</v>
-          </cell>
-          <cell r="I6">
-            <v>2685</v>
-          </cell>
-          <cell r="J6">
-            <v>43251</v>
-          </cell>
-          <cell r="K6">
-            <v>10525875</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="Sheet1"/>
       <sheetName val="Sheet2"/>
       <sheetName val="Sheet3"/>
-      <sheetName val="PROPIS"/>
     </sheetNames>
     <definedNames>
       <definedName name="prop"/>
     </definedNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1838,7 +1759,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1910,7 +1831,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2067,681 +1988,657 @@
   <dimension ref="B1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="0.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="4.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="21.85546875" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="0.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
-      <c r="C1" s="174" t="s">
+      <c r="C1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="174"/>
-      <c r="E1" s="2">
-        <f>'[1]Reg.List'!I6</f>
-        <v>2685</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="175">
-        <f>'[1]Reg.List'!J6</f>
-        <v>43251</v>
-      </c>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="165"/>
+      <c r="I1" s="165"/>
+      <c r="J1" s="165"/>
+      <c r="K1" s="165"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="2:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5"/>
-      <c r="C3" s="61" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="6" t="str">
-        <f>'[1]Reg.List'!E6</f>
-        <v>SOCIE 2017/096</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="60"/>
+      <c r="E3" s="164"/>
+      <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="175">
-        <f>'[1]Reg.List'!G6</f>
-        <v>42963</v>
-      </c>
-      <c r="H3" s="175"/>
+      <c r="G3" s="165"/>
+      <c r="H3" s="165"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:12" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="176"/>
-      <c r="J4" s="176"/>
-      <c r="K4" s="176"/>
-      <c r="L4" s="176"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
     </row>
     <row r="5" spans="2:12" ht="5.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="10"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="177" t="s">
+      <c r="C6" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="177"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="11" t="s">
+      <c r="D6" s="57"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="178"/>
-      <c r="H6" s="178"/>
-      <c r="I6" s="178"/>
-      <c r="J6" s="178"/>
-      <c r="K6" s="178"/>
-      <c r="L6" s="13"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="172" t="s">
+      <c r="C7" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="172"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="11" t="s">
+      <c r="D7" s="62"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="161"/>
-      <c r="H7" s="161"/>
-      <c r="I7" s="161"/>
-      <c r="J7" s="161"/>
-      <c r="K7" s="161"/>
-      <c r="L7" s="13"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="172" t="s">
+      <c r="C8" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="172"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="11" t="s">
+      <c r="D8" s="62"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="161"/>
-      <c r="H8" s="161"/>
-      <c r="I8" s="161"/>
-      <c r="J8" s="161"/>
-      <c r="K8" s="161"/>
-      <c r="L8" s="13"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="160" t="s">
+      <c r="C9" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="160"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="11" t="s">
+      <c r="D9" s="64"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="161"/>
-      <c r="H9" s="161"/>
-      <c r="I9" s="161"/>
-      <c r="J9" s="161"/>
-      <c r="K9" s="161"/>
-      <c r="L9" s="13"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="172" t="s">
+      <c r="C10" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="172"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11" t="s">
+      <c r="D10" s="62"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="161"/>
-      <c r="H10" s="161"/>
-      <c r="I10" s="161"/>
-      <c r="J10" s="161"/>
-      <c r="K10" s="161"/>
-      <c r="L10" s="13"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="160" t="s">
+      <c r="C11" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="160"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="11" t="s">
+      <c r="D11" s="64"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="161"/>
-      <c r="H11" s="161"/>
-      <c r="I11" s="161"/>
-      <c r="J11" s="161"/>
-      <c r="K11" s="161"/>
-      <c r="L11" s="13"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="11"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="173" t="s">
+      <c r="C12" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="173"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="11" t="s">
+      <c r="D12" s="65"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="161"/>
-      <c r="H12" s="161"/>
-      <c r="I12" s="161"/>
-      <c r="J12" s="161"/>
-      <c r="K12" s="161"/>
-      <c r="L12" s="13"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="160" t="s">
+      <c r="C13" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="160"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="11" t="s">
+      <c r="D13" s="64"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="161"/>
-      <c r="H13" s="161"/>
-      <c r="I13" s="161"/>
-      <c r="J13" s="161"/>
-      <c r="K13" s="161"/>
-      <c r="L13" s="13"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="11"/>
     </row>
     <row r="14" spans="2:12" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="16"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="14"/>
     </row>
     <row r="15" spans="2:12" ht="6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:12" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="162" t="s">
+      <c r="B16" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="163"/>
-      <c r="D16" s="129" t="s">
+      <c r="C16" s="67"/>
+      <c r="D16" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="166" t="s">
+      <c r="E16" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="162" t="s">
+      <c r="F16" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="168" t="s">
+      <c r="G16" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="170" t="s">
+      <c r="H16" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="171"/>
-      <c r="J16" s="171" t="s">
+      <c r="I16" s="77"/>
+      <c r="J16" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="K16" s="163"/>
-      <c r="L16" s="129" t="s">
+      <c r="K16" s="67"/>
+      <c r="L16" s="70" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="164"/>
-      <c r="C17" s="165"/>
-      <c r="D17" s="130"/>
-      <c r="E17" s="167"/>
-      <c r="F17" s="164"/>
-      <c r="G17" s="169"/>
-      <c r="H17" s="17" t="s">
+      <c r="B17" s="68"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="I17" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="L17" s="130"/>
+      <c r="L17" s="71"/>
     </row>
     <row r="18" spans="2:14" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="131">
+      <c r="B18" s="78">
         <v>1</v>
       </c>
-      <c r="C18" s="132"/>
-      <c r="D18" s="21">
+      <c r="C18" s="79"/>
+      <c r="D18" s="19">
         <v>2</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="20">
         <v>3</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="21">
         <v>4</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="22">
         <v>5</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="23">
         <v>6</v>
       </c>
-      <c r="I18" s="26">
+      <c r="I18" s="24">
         <v>7</v>
       </c>
-      <c r="J18" s="26">
+      <c r="J18" s="24">
         <v>8</v>
       </c>
-      <c r="K18" s="27">
+      <c r="K18" s="25">
         <v>9</v>
       </c>
-      <c r="L18" s="21">
+      <c r="L18" s="19">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="133" t="s">
+      <c r="B19" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="134"/>
-      <c r="D19" s="135" t="s">
+      <c r="C19" s="81"/>
+      <c r="D19" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="138"/>
-      <c r="F19" s="141">
-        <f>'[1]Reg.List'!K6</f>
-        <v>10525875</v>
-      </c>
-      <c r="G19" s="144">
+      <c r="E19" s="85"/>
+      <c r="F19" s="170"/>
+      <c r="G19" s="170">
         <f>F19</f>
-        <v>10525875</v>
-      </c>
-      <c r="H19" s="147" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="148"/>
-      <c r="J19" s="153" t="s">
+      <c r="I19" s="89"/>
+      <c r="J19" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="K19" s="154"/>
-      <c r="L19" s="159" t="s">
+      <c r="K19" s="95"/>
+      <c r="L19" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="N19" s="28"/>
+      <c r="N19" s="26"/>
     </row>
     <row r="20" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="106" t="str">
-        <f>'[1]Reg.List'!B6</f>
-        <v>SHOKHUJAEV IBROKHIMKHUJA</v>
-      </c>
-      <c r="C20" s="107"/>
-      <c r="D20" s="136"/>
-      <c r="E20" s="139"/>
-      <c r="F20" s="142"/>
-      <c r="G20" s="145"/>
-      <c r="H20" s="149"/>
-      <c r="I20" s="150"/>
-      <c r="J20" s="155"/>
-      <c r="K20" s="156"/>
-      <c r="L20" s="108"/>
+      <c r="B20" s="166"/>
+      <c r="C20" s="167"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="171"/>
+      <c r="G20" s="171"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="96"/>
+      <c r="K20" s="97"/>
+      <c r="L20" s="101"/>
     </row>
     <row r="21" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="30" t="str">
-        <f>'[1]Reg.List'!C6</f>
-        <v>SOCIE</v>
-      </c>
-      <c r="D21" s="136"/>
-      <c r="E21" s="139"/>
-      <c r="F21" s="142"/>
-      <c r="G21" s="145"/>
-      <c r="H21" s="149"/>
-      <c r="I21" s="150"/>
-      <c r="J21" s="155"/>
-      <c r="K21" s="156"/>
-      <c r="L21" s="108" t="s">
+      <c r="C21" s="28"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="171"/>
+      <c r="G21" s="171"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="91"/>
+      <c r="J21" s="96"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="101" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="110" t="str">
-        <f>'[1]Reg.List'!D5</f>
-        <v xml:space="preserve"> за II-семестр 2017 / 2018 учеб. год</v>
-      </c>
-      <c r="C22" s="111"/>
-      <c r="D22" s="137"/>
-      <c r="E22" s="140"/>
-      <c r="F22" s="143"/>
-      <c r="G22" s="146"/>
-      <c r="H22" s="151"/>
-      <c r="I22" s="152"/>
-      <c r="J22" s="157"/>
-      <c r="K22" s="158"/>
-      <c r="L22" s="109"/>
+      <c r="B22" s="168"/>
+      <c r="C22" s="169"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="172"/>
+      <c r="G22" s="172"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="93"/>
+      <c r="J22" s="98"/>
+      <c r="K22" s="99"/>
+      <c r="L22" s="104"/>
     </row>
     <row r="23" spans="2:14" ht="9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="112"/>
-      <c r="C23" s="113"/>
-      <c r="D23" s="113"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="113"/>
-      <c r="G23" s="113"/>
-      <c r="H23" s="113"/>
-      <c r="I23" s="113"/>
-      <c r="J23" s="113"/>
-      <c r="K23" s="113"/>
-      <c r="L23" s="114"/>
+      <c r="B23" s="105"/>
+      <c r="C23" s="106"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="106"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="106"/>
+      <c r="H23" s="106"/>
+      <c r="I23" s="106"/>
+      <c r="J23" s="106"/>
+      <c r="K23" s="106"/>
+      <c r="L23" s="107"/>
     </row>
     <row r="24" spans="2:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="115" t="s">
+      <c r="B24" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="98"/>
-      <c r="D24" s="117" t="s">
+      <c r="C24" s="109"/>
+      <c r="D24" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="119"/>
-      <c r="F24" s="121">
+      <c r="E24" s="114"/>
+      <c r="F24" s="175">
         <f>F19</f>
-        <v>10525875</v>
-      </c>
-      <c r="G24" s="123">
+        <v>0</v>
+      </c>
+      <c r="G24" s="173">
         <f>G19</f>
-        <v>10525875</v>
-      </c>
-      <c r="H24" s="125" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="I24" s="126"/>
-      <c r="J24" s="97" t="s">
+      <c r="I24" s="117"/>
+      <c r="J24" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="98"/>
-      <c r="L24" s="31" t="s">
+      <c r="K24" s="109"/>
+      <c r="L24" s="29" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="116"/>
-      <c r="C25" s="100"/>
-      <c r="D25" s="118"/>
-      <c r="E25" s="120"/>
-      <c r="F25" s="122"/>
-      <c r="G25" s="124"/>
-      <c r="H25" s="127"/>
-      <c r="I25" s="128"/>
-      <c r="J25" s="99"/>
-      <c r="K25" s="100"/>
-      <c r="L25" s="32" t="s">
+      <c r="B25" s="110"/>
+      <c r="C25" s="111"/>
+      <c r="D25" s="113"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="176"/>
+      <c r="G25" s="174"/>
+      <c r="H25" s="118"/>
+      <c r="I25" s="119"/>
+      <c r="J25" s="121"/>
+      <c r="K25" s="111"/>
+      <c r="L25" s="30" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:14" ht="7.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
-      <c r="L26" s="36"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="34"/>
     </row>
     <row r="27" spans="2:14" ht="4.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="101"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
+      <c r="B27" s="102"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
     </row>
     <row r="28" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="102"/>
-      <c r="I28" s="102"/>
-      <c r="J28" s="102"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="122"/>
+      <c r="I28" s="122"/>
+      <c r="J28" s="122"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="103" t="e">
-        <f ca="1">[2]!prop(F24)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D29" s="103"/>
-      <c r="E29" s="103"/>
-      <c r="F29" s="103"/>
-      <c r="G29" s="103"/>
-      <c r="H29" s="103"/>
-      <c r="I29" s="103"/>
-      <c r="J29" s="103"/>
-      <c r="K29" s="103"/>
-      <c r="L29" s="103"/>
+      <c r="C29" s="150" t="str">
+        <f>[1]!prop(F24)</f>
+        <v>Сум 00 тийин</v>
+      </c>
+      <c r="D29" s="150"/>
+      <c r="E29" s="150"/>
+      <c r="F29" s="150"/>
+      <c r="G29" s="150"/>
+      <c r="H29" s="150"/>
+      <c r="I29" s="150"/>
+      <c r="J29" s="150"/>
+      <c r="K29" s="150"/>
+      <c r="L29" s="150"/>
     </row>
     <row r="30" spans="2:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="37"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="40" t="s">
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
     </row>
     <row r="32" spans="2:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="104" t="s">
+      <c r="C32" s="35"/>
+      <c r="D32" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="101"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="43" t="s">
+      <c r="E32" s="102"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="44"/>
-      <c r="N32" s="45"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
+      <c r="N32" s="43"/>
     </row>
     <row r="33" spans="2:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="42" t="s">
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
     </row>
     <row r="34" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="37"/>
-      <c r="D34" s="101" t="s">
+      <c r="C34" s="35"/>
+      <c r="D34" s="151" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="101"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="105" t="s">
+      <c r="E34" s="151"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="H34" s="105"/>
-      <c r="I34" s="105"/>
-      <c r="J34" s="105"/>
-      <c r="K34" s="105"/>
-      <c r="L34" s="105"/>
+      <c r="H34" s="103"/>
+      <c r="I34" s="103"/>
+      <c r="J34" s="103"/>
+      <c r="K34" s="103"/>
+      <c r="L34" s="103"/>
     </row>
     <row r="35" spans="2:12" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
-      <c r="J35" s="46"/>
-      <c r="K35" s="46"/>
-      <c r="L35" s="46"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B36" s="42"/>
-      <c r="H36" s="92" t="s">
+      <c r="B36" s="40"/>
+      <c r="H36" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="I36" s="92"/>
-      <c r="J36" s="92"/>
-      <c r="K36" s="92"/>
-      <c r="L36" s="92"/>
+      <c r="I36" s="124"/>
+      <c r="J36" s="124"/>
+      <c r="K36" s="124"/>
+      <c r="L36" s="124"/>
     </row>
     <row r="37" spans="2:12" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="93"/>
-      <c r="C37" s="93"/>
-      <c r="H37" s="94"/>
-      <c r="I37" s="94"/>
-      <c r="J37" s="94"/>
-      <c r="K37" s="94"/>
-      <c r="L37" s="94"/>
+      <c r="B37" s="125"/>
+      <c r="C37" s="125"/>
+      <c r="H37" s="126"/>
+      <c r="I37" s="126"/>
+      <c r="J37" s="126"/>
+      <c r="K37" s="126"/>
+      <c r="L37" s="126"/>
     </row>
     <row r="38" spans="2:12" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="48"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
     </row>
     <row r="39" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="95" t="s">
+      <c r="B40" s="127" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="95"/>
-      <c r="D40" s="95"/>
-      <c r="E40" s="95"/>
-      <c r="F40" s="95"/>
-      <c r="G40" s="49">
+      <c r="C40" s="127"/>
+      <c r="D40" s="127"/>
+      <c r="E40" s="127"/>
+      <c r="F40" s="127"/>
+      <c r="G40" s="146">
         <f>E1</f>
-        <v>2685</v>
+        <v>0</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2750,257 +2647,242 @@
       <c r="L40" s="1"/>
     </row>
     <row r="41" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="50"/>
-      <c r="C41" s="61" t="s">
+      <c r="B41" s="47"/>
+      <c r="C41" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="61"/>
-      <c r="E41" s="51" t="str">
+      <c r="D41" s="60"/>
+      <c r="E41" s="149">
         <f>E3</f>
-        <v>SOCIE 2017/096</v>
-      </c>
-      <c r="F41" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G41" s="96">
+      <c r="G41" s="145">
         <f>G3</f>
-        <v>42963</v>
-      </c>
-      <c r="H41" s="96"/>
+        <v>0</v>
+      </c>
+      <c r="H41" s="145"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="50"/>
-      <c r="L41" s="50"/>
+      <c r="K41" s="47"/>
+      <c r="L41" s="47"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B43" s="52" t="s">
+      <c r="B43" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="52"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="52"/>
-      <c r="I43" s="52"/>
-      <c r="J43" s="83">
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="144"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="147">
         <f>G1</f>
-        <v>43251</v>
-      </c>
-      <c r="K43" s="84"/>
-      <c r="L43" s="84"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="148"/>
+      <c r="L43" s="148"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B45" s="85" t="s">
+      <c r="B45" s="128" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="85"/>
-      <c r="D45" s="85"/>
-      <c r="E45" s="85"/>
-      <c r="F45" s="85"/>
-      <c r="G45" s="85"/>
-      <c r="H45" s="85"/>
-      <c r="I45" s="85"/>
-      <c r="J45" s="85"/>
-      <c r="K45" s="85"/>
-      <c r="L45" s="85"/>
+      <c r="C45" s="128"/>
+      <c r="D45" s="128"/>
+      <c r="E45" s="128"/>
+      <c r="F45" s="128"/>
+      <c r="G45" s="128"/>
+      <c r="H45" s="128"/>
+      <c r="I45" s="128"/>
+      <c r="J45" s="128"/>
+      <c r="K45" s="128"/>
+      <c r="L45" s="128"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B46" s="53" t="s">
+      <c r="B46" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="53"/>
-      <c r="D46" s="86"/>
-      <c r="E46" s="86"/>
-      <c r="F46" s="86"/>
-      <c r="G46" s="86"/>
-      <c r="H46" s="86"/>
-      <c r="I46" s="86"/>
-      <c r="J46" s="86"/>
-      <c r="K46" s="86"/>
-      <c r="L46" s="86"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="129"/>
+      <c r="E46" s="129"/>
+      <c r="F46" s="129"/>
+      <c r="G46" s="129"/>
+      <c r="H46" s="129"/>
+      <c r="I46" s="129"/>
+      <c r="J46" s="129"/>
+      <c r="K46" s="129"/>
+      <c r="L46" s="129"/>
     </row>
     <row r="47" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="87" t="s">
+      <c r="B47" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="87"/>
-      <c r="D47" s="87"/>
-      <c r="E47" s="87"/>
-      <c r="F47" s="87"/>
-      <c r="G47" s="87"/>
-      <c r="H47" s="87"/>
-      <c r="I47" s="87"/>
-      <c r="J47" s="87"/>
-      <c r="K47" s="87"/>
-      <c r="L47" s="87"/>
+      <c r="C47" s="130"/>
+      <c r="D47" s="130"/>
+      <c r="E47" s="130"/>
+      <c r="F47" s="130"/>
+      <c r="G47" s="130"/>
+      <c r="H47" s="130"/>
+      <c r="I47" s="130"/>
+      <c r="J47" s="130"/>
+      <c r="K47" s="130"/>
+      <c r="L47" s="130"/>
     </row>
     <row r="48" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="88" t="s">
+      <c r="B49" s="131" t="s">
         <v>53</v>
       </c>
-      <c r="C49" s="89"/>
-      <c r="D49" s="89"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="90"/>
-      <c r="G49" s="88" t="s">
+      <c r="C49" s="132"/>
+      <c r="D49" s="132"/>
+      <c r="E49" s="132"/>
+      <c r="F49" s="133"/>
+      <c r="G49" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="H49" s="89"/>
-      <c r="I49" s="89" t="s">
+      <c r="H49" s="132"/>
+      <c r="I49" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="J49" s="89"/>
-      <c r="K49" s="91"/>
-      <c r="L49" s="54"/>
+      <c r="J49" s="132"/>
+      <c r="K49" s="134"/>
+      <c r="L49" s="50"/>
     </row>
     <row r="50" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="55" t="s">
+      <c r="B50" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="64" t="str">
+      <c r="C50" s="152">
         <f>B20</f>
-        <v>SHOKHUJAEV IBROKHIMKHUJA</v>
-      </c>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="152"/>
+      <c r="E50" s="152"/>
+      <c r="F50" s="153"/>
+      <c r="G50" s="136" t="s">
         <v>31</v>
       </c>
-      <c r="H50" s="67"/>
-      <c r="I50" s="70">
+      <c r="H50" s="137"/>
+      <c r="I50" s="158">
         <f>F19</f>
-        <v>10525875</v>
-      </c>
-      <c r="J50" s="71"/>
-      <c r="K50" s="72"/>
-      <c r="L50" s="56"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="159"/>
+      <c r="K50" s="160"/>
+      <c r="L50" s="52"/>
     </row>
     <row r="51" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="76" t="s">
+      <c r="B51" s="154" t="s">
         <v>56</v>
       </c>
-      <c r="C51" s="77"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="77"/>
-      <c r="F51" s="78"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="69"/>
-      <c r="I51" s="73"/>
-      <c r="J51" s="74"/>
-      <c r="K51" s="75"/>
+      <c r="C51" s="155"/>
+      <c r="D51" s="155"/>
+      <c r="E51" s="155"/>
+      <c r="F51" s="156"/>
+      <c r="G51" s="138"/>
+      <c r="H51" s="139"/>
+      <c r="I51" s="161"/>
+      <c r="J51" s="162"/>
+      <c r="K51" s="163"/>
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="79"/>
-      <c r="C52" s="80"/>
-      <c r="D52" s="80"/>
-      <c r="E52" s="80"/>
-      <c r="F52" s="81"/>
-      <c r="G52" s="79"/>
-      <c r="H52" s="80"/>
-      <c r="I52" s="80"/>
-      <c r="J52" s="80"/>
-      <c r="K52" s="82"/>
-      <c r="L52" s="57"/>
+      <c r="B52" s="140"/>
+      <c r="C52" s="141"/>
+      <c r="D52" s="141"/>
+      <c r="E52" s="141"/>
+      <c r="F52" s="142"/>
+      <c r="G52" s="140"/>
+      <c r="H52" s="141"/>
+      <c r="I52" s="141"/>
+      <c r="J52" s="141"/>
+      <c r="K52" s="143"/>
+      <c r="L52" s="53"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B54" s="61" t="s">
+      <c r="B54" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="61"/>
-      <c r="D54" s="62" t="e">
-        <f ca="1">C29</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E54" s="62"/>
-      <c r="F54" s="62"/>
-      <c r="G54" s="62"/>
-      <c r="H54" s="62"/>
-      <c r="I54" s="62"/>
-      <c r="J54" s="62"/>
-      <c r="K54" s="62"/>
-      <c r="L54" s="62"/>
+      <c r="C54" s="60"/>
+      <c r="D54" s="157" t="str">
+        <f>C29</f>
+        <v>Сум 00 тийин</v>
+      </c>
+      <c r="E54" s="157"/>
+      <c r="F54" s="157"/>
+      <c r="G54" s="157"/>
+      <c r="H54" s="157"/>
+      <c r="I54" s="157"/>
+      <c r="J54" s="157"/>
+      <c r="K54" s="157"/>
+      <c r="L54" s="157"/>
     </row>
     <row r="55" spans="2:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="63" t="s">
+      <c r="B55" s="135" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="63"/>
-      <c r="D55" s="63"/>
-      <c r="E55" s="63"/>
-      <c r="F55" s="63"/>
-      <c r="G55" s="63"/>
-      <c r="H55" s="63"/>
-      <c r="I55" s="63"/>
-      <c r="J55" s="63"/>
-      <c r="K55" s="63"/>
-      <c r="L55" s="63"/>
+      <c r="C55" s="135"/>
+      <c r="D55" s="135"/>
+      <c r="E55" s="135"/>
+      <c r="F55" s="135"/>
+      <c r="G55" s="135"/>
+      <c r="H55" s="135"/>
+      <c r="I55" s="135"/>
+      <c r="J55" s="135"/>
+      <c r="K55" s="135"/>
+      <c r="L55" s="135"/>
     </row>
     <row r="58" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="C58" s="58" t="s">
+      <c r="C58" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="D58" s="59"/>
-      <c r="E58" s="59"/>
-      <c r="G58" s="60" t="s">
+      <c r="D58" s="55"/>
+      <c r="E58" s="55"/>
+      <c r="G58" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="H58" s="46"/>
-      <c r="I58" s="46"/>
-      <c r="J58" s="46"/>
-      <c r="K58" s="46"/>
+      <c r="H58" s="44"/>
+      <c r="I58" s="44"/>
+      <c r="J58" s="44"/>
+      <c r="K58" s="44"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C59" s="28" t="s">
+      <c r="C59" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="H59" s="4" t="s">
+      <c r="H59" s="3" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="H19:I22"/>
-    <mergeCell ref="J19:K22"/>
-    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="B55:L55"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="G50:H51"/>
+    <mergeCell ref="I50:K51"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="G52:K52"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:L54"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="D46:L46"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="B40:F40"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="G34:L34"/>
     <mergeCell ref="B20:C20"/>
@@ -3017,29 +2899,44 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="H28:J28"/>
     <mergeCell ref="C29:L29"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="D46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:K49"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:L54"/>
-    <mergeCell ref="B55:L55"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="G50:H51"/>
-    <mergeCell ref="I50:K51"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="G52:K52"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H19:I22"/>
+    <mergeCell ref="J19:K22"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B4:L4"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="11" scale="53" orientation="portrait" r:id="rId1"/>

</xml_diff>